<commit_message>
S03P31D201-1 | ERD, API 리스트
</commit_message>
<xml_diff>
--- a/backend/API 리스트.xlsx
+++ b/backend/API 리스트.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\SSAFY\자율\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\multicampus\SSAFY\자율\자율\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>int : 코스 데이터(integer, 0 ~ 3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/tour/place/&lt;int:&gt;/mission/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,10 +78,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/calendar/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기존 여행 일정 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -98,10 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/calendar/date/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,10 +154,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/review/create/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>title, content</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,10 +182,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/place/custom/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/tour/&lt;int:&gt;/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -218,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/place/custom/&lt;int:&gt;/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int : 커스텀 미션 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -262,22 +238,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/calendar/date/?date=abc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/tour/calendar/date/place/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>patch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/tour/place/&lt;int:&gt;/custom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int : user_pk</t>
   </si>
   <si>
@@ -324,10 +288,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>사용자 정보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>사용자 정보 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -352,15 +312,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0 : 미방문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 : 방문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 : 방문예정</t>
+    <t>int : 코스 데이터(integer)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/place/&lt;int:&gt;/custom/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/place/&lt;int:&gt;/custom/&lt;int:&gt;/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 정보(프로필 페이지)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 : 방문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 : 방문예정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/&lt;int:&gt;/calendar/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/&lt;int:&gt;/calendar/date/?date=abc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/&lt;int:&gt;/calendar/date/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/tour/&lt;int:&gt;/calendar/date/place/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코멘트 정보 get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,15 +385,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -518,22 +530,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -554,29 +557,74 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -859,11 +907,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I34"/>
+  <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -874,61 +920,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="27" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>66</v>
+      <c r="A3" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -938,106 +992,104 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="11"/>
+      <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="11"/>
+      <c r="B8" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="11"/>
+      <c r="B9" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>84</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
@@ -1045,57 +1097,57 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="8"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="8"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -1104,192 +1156,194 @@
         <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="8"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" s="8"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="E24" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="B27" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" s="8"/>
-      <c r="B23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="9"/>
-      <c r="B26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>9</v>
@@ -1297,120 +1351,134 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29" s="8"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="11"/>
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30" s="8"/>
-      <c r="B30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32" s="8"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>9</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="11"/>
+      <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A33" s="8"/>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" s="11"/>
+      <c r="B34" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="9"/>
-      <c r="B34" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="12"/>
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="A27:A35"/>
     <mergeCell ref="A3:A10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
S03P31D201-1 | ERD 및 API 리스트 수정
</commit_message>
<xml_diff>
--- a/backend/API 리스트.xlsx
+++ b/backend/API 리스트.xlsx
@@ -265,18 +265,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/rest-auth/registration/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>username, password1, password2, email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>username, email, password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>token</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,6 +349,18 @@
   </si>
   <si>
     <t>수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, password1, password2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email, password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rest-auth/signup/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -570,62 +570,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,7 +909,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -920,53 +922,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="27" t="s">
-        <v>83</v>
+      <c r="G2" s="22"/>
+      <c r="H2" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="27" t="s">
-        <v>84</v>
+        <v>60</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="11"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>58</v>
       </c>
@@ -974,13 +976,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="11"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>59</v>
       </c>
@@ -992,9 +994,9 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="11"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>9</v>
@@ -1004,13 +1006,13 @@
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>53</v>
@@ -1019,46 +1021,46 @@
         <v>55</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="24"/>
+      <c r="B8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="24"/>
+      <c r="B9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="25"/>
+      <c r="B10" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="11"/>
-      <c r="B8" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="12"/>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -1068,18 +1070,18 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1089,7 +1091,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
@@ -1097,7 +1099,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="11"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1115,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="11"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1129,9 +1131,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1145,9 +1147,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="11"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>4</v>
@@ -1161,9 +1163,9 @@
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="11"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -1177,9 +1179,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" s="11"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>53</v>
@@ -1193,9 +1195,9 @@
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="12"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>50</v>
@@ -1209,137 +1211,137 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="27"/>
+      <c r="B21" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="27"/>
+      <c r="B22" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="27"/>
+      <c r="B23" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="27"/>
+      <c r="B24" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="19"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="D24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="27"/>
+      <c r="B25" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="28"/>
+      <c r="B26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="D26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="19"/>
-    </row>
-    <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -1355,7 +1357,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28" s="11"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1371,7 +1373,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29" s="11"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1387,7 +1389,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30" s="11"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1403,7 +1405,7 @@
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31" s="11"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1417,21 +1419,21 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32" s="11"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A33" s="11"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
@@ -1445,21 +1447,21 @@
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A34" s="11"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="24"/>
+      <c r="B34" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23" t="s">
+      <c r="D34" s="17"/>
+      <c r="E34" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="12"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="8" t="s">
         <v>47</v>
       </c>

</xml_diff>